<commit_message>
Add common years filtering, update conclusions
</commit_message>
<xml_diff>
--- a/Мазяр - Таблица для расчетного задания.xlsx
+++ b/Мазяр - Таблица для расчетного задания.xlsx
@@ -451,15 +451,15 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="11.0"/>
       <color rgb="FFCCCCCC"/>
       <name val="&quot;Segoe WPC&quot;"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -984,7 +984,10 @@
     <xf borderId="15" fillId="5" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="5" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="5" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1023,10 +1026,7 @@
     <xf borderId="19" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1035,10 +1035,10 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="22" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1447,239 +1447,284 @@
       <c r="K5" s="23"/>
       <c r="L5" s="24"/>
       <c r="M5" s="27"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
     </row>
     <row r="6" ht="18.0" customHeight="1">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="30">
         <v>8.583066</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="31">
         <v>19.454127</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="32">
         <v>4.984899</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="33">
         <v>8.218528</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="34">
         <v>11.437482</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="35">
         <v>2.786864</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="36">
         <v>6.373114</v>
       </c>
-      <c r="I6" s="36">
+      <c r="I6" s="37">
         <v>4.217187</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="38">
         <v>1.879986</v>
       </c>
-      <c r="K6" s="38">
+      <c r="K6" s="39">
         <v>4.502742</v>
       </c>
-      <c r="L6" s="39">
+      <c r="L6" s="40">
         <v>2.295294</v>
       </c>
-      <c r="M6" s="40">
+      <c r="M6" s="41">
         <v>1.301896</v>
       </c>
+      <c r="O6" s="28"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="42"/>
+      <c r="V6" s="42"/>
+      <c r="W6" s="42"/>
+      <c r="X6" s="42"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="42"/>
+      <c r="AA6" s="42"/>
+      <c r="AB6" s="42"/>
+      <c r="AC6" s="42"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="30">
         <v>1.48856</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="31">
         <v>0.821218</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="32">
         <v>1.065712</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="33">
         <v>1.499924</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="34">
         <v>0.66618</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="35">
         <v>1.071046</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="36">
         <v>1.230029</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="37">
         <v>0.876551</v>
       </c>
-      <c r="J7" s="37">
+      <c r="J7" s="38">
         <v>0.917662</v>
       </c>
-      <c r="K7" s="38">
+      <c r="K7" s="39">
         <v>1.260693</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="40">
         <v>0.810748</v>
       </c>
-      <c r="M7" s="40">
+      <c r="M7" s="41">
         <v>0.86754</v>
       </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="41"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="41"/>
-      <c r="AC7" s="41"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="43"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="43"/>
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="43"/>
+      <c r="AA7" s="43"/>
+      <c r="AB7" s="43"/>
+      <c r="AC7" s="43"/>
     </row>
     <row r="8" ht="18.0" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="30">
         <v>2.237448</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="31">
         <v>1.251424</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="32">
         <v>1.473698</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="33">
         <v>2.313703</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="34">
         <v>1.119397</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="35">
         <v>1.926053</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="36">
         <v>2.178903</v>
       </c>
-      <c r="I8" s="36">
+      <c r="I8" s="37">
         <v>1.180631</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="38">
         <v>1.373545</v>
       </c>
-      <c r="K8" s="38">
+      <c r="K8" s="39">
         <v>1.979017</v>
       </c>
-      <c r="L8" s="39">
+      <c r="L8" s="40">
         <v>1.186271</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8" s="41">
         <v>0.86608</v>
       </c>
-      <c r="O8" s="41"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="42"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="42"/>
-      <c r="AC8" s="42"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="43"/>
+      <c r="Y8" s="43"/>
+      <c r="Z8" s="43"/>
+      <c r="AA8" s="43"/>
+      <c r="AB8" s="43"/>
+      <c r="AC8" s="43"/>
     </row>
     <row r="9" ht="18.0" customHeight="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="30">
         <v>4.422488</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="31">
         <v>2.078711</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="32">
         <v>1.806207</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="33">
         <v>3.111248</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="34">
         <v>2.575423</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="35">
         <v>2.768973</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="36">
         <v>3.258184</v>
       </c>
-      <c r="I9" s="36">
+      <c r="I9" s="37">
         <v>3.159957</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="38">
         <v>3.225244</v>
       </c>
-      <c r="K9" s="38">
+      <c r="K9" s="39">
         <v>3.579953</v>
       </c>
-      <c r="L9" s="39">
+      <c r="L9" s="40">
         <v>3.617904</v>
       </c>
-      <c r="M9" s="40">
+      <c r="M9" s="41">
         <v>3.316558</v>
       </c>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="43"/>
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="43"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="43"/>
+      <c r="AC9" s="43"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="30">
         <v>1.692445</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="31">
         <v>1.324348</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="32">
         <v>3.168808</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="33">
         <v>1.740041</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="34">
         <v>1.970559</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="35">
         <v>3.579349</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="36">
         <v>1.601963</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="37">
         <v>2.41023</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="38">
         <v>3.919621</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="39">
         <v>1.816287</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="40">
         <v>3.388568</v>
       </c>
-      <c r="M10" s="40">
+      <c r="M10" s="41">
         <v>3.772256</v>
       </c>
       <c r="O10" s="43"/>
@@ -1702,40 +1747,40 @@
       <c r="A11" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="30">
         <v>2.276715</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="31">
         <v>1.20146</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="32">
         <v>4.166386</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="33">
         <v>2.138156</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="34">
         <v>1.572528</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="35">
         <v>3.329795</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="36">
         <v>1.514135</v>
       </c>
-      <c r="I11" s="36">
+      <c r="I11" s="37">
         <v>2.086548</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="38">
         <v>3.355746</v>
       </c>
-      <c r="K11" s="38">
+      <c r="K11" s="39">
         <v>1.709517</v>
       </c>
-      <c r="L11" s="39">
+      <c r="L11" s="40">
         <v>2.72599</v>
       </c>
-      <c r="M11" s="40">
+      <c r="M11" s="41">
         <v>3.897908</v>
       </c>
       <c r="O11" s="43"/>
@@ -1758,40 +1803,40 @@
       <c r="A12" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="30">
         <v>5.062763</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="31">
         <v>2.541158</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="32">
         <v>1.041901</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="33">
         <v>4.01015</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="34">
         <v>2.329591</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="35">
         <v>0.979839</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H12" s="36">
         <v>2.858716</v>
       </c>
-      <c r="I12" s="36">
+      <c r="I12" s="37">
         <v>1.435468</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="38">
         <v>0.553907</v>
       </c>
-      <c r="K12" s="38">
+      <c r="K12" s="39">
         <v>2.448844</v>
       </c>
-      <c r="L12" s="39">
+      <c r="L12" s="40">
         <v>1.001189</v>
       </c>
-      <c r="M12" s="40">
+      <c r="M12" s="41">
         <v>0.33848</v>
       </c>
     </row>
@@ -1803,37 +1848,37 @@
         <v>1.869431</v>
       </c>
       <c r="C13" s="48">
-        <v>3.344194</v>
+        <v>1.350047</v>
       </c>
       <c r="D13" s="49">
-        <v>1.272368</v>
+        <v>1.052926</v>
       </c>
       <c r="E13" s="50">
         <v>1.679368</v>
       </c>
       <c r="F13" s="51">
-        <v>3.296652</v>
+        <v>1.066924</v>
       </c>
       <c r="G13" s="52">
-        <v>1.131721</v>
+        <v>0.89419</v>
       </c>
       <c r="H13" s="53">
         <v>1.669925</v>
       </c>
       <c r="I13" s="54">
-        <v>2.083181</v>
+        <v>1.086024</v>
       </c>
       <c r="J13" s="55">
-        <v>0.692635</v>
+        <v>0.815458</v>
       </c>
       <c r="K13" s="56">
         <v>1.524963</v>
       </c>
       <c r="L13" s="57">
-        <v>1.303579</v>
+        <v>0.950791</v>
       </c>
       <c r="M13" s="58">
-        <v>0.397365</v>
+        <v>0.430746</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1857,40 +1902,40 @@
       <c r="A15" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="30">
         <v>1.0</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="31">
         <v>1.0</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="32">
         <v>1.0</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="33">
         <v>1.0</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="34">
         <v>1.0</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="35">
         <v>1.0</v>
       </c>
-      <c r="H15" s="35">
+      <c r="H15" s="36">
         <v>1.0</v>
       </c>
-      <c r="I15" s="36">
+      <c r="I15" s="37">
         <v>1.0</v>
       </c>
-      <c r="J15" s="37">
+      <c r="J15" s="38">
         <v>1.0</v>
       </c>
-      <c r="K15" s="38">
+      <c r="K15" s="39">
         <v>1.0</v>
       </c>
-      <c r="L15" s="39">
+      <c r="L15" s="40">
         <v>1.0</v>
       </c>
-      <c r="M15" s="40">
+      <c r="M15" s="41">
         <v>1.0</v>
       </c>
       <c r="O15" s="43"/>
@@ -1913,40 +1958,40 @@
       <c r="A16" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="30">
         <v>0.876394</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="31">
         <v>0.966277</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="32">
         <v>0.959345</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="33">
         <v>0.866588</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="34">
         <v>0.910443</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="35">
         <v>0.870591</v>
       </c>
-      <c r="H16" s="35">
+      <c r="H16" s="36">
         <v>0.845144</v>
       </c>
-      <c r="I16" s="36">
+      <c r="I16" s="37">
         <v>0.882838</v>
       </c>
-      <c r="J16" s="37">
+      <c r="J16" s="38">
         <v>0.928166</v>
       </c>
-      <c r="K16" s="38">
+      <c r="K16" s="39">
         <v>0.817748</v>
       </c>
-      <c r="L16" s="39">
+      <c r="L16" s="40">
         <v>0.776272</v>
       </c>
-      <c r="M16" s="40">
+      <c r="M16" s="41">
         <v>0.914182</v>
       </c>
       <c r="O16" s="43"/>
@@ -1969,40 +2014,40 @@
       <c r="A17" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="30">
         <v>-0.537477</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="31">
         <v>0.336547</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="32">
         <v>0.054809</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="33">
         <v>-0.527235</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="34">
         <v>-0.071834</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="35">
         <v>-0.128577</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="36">
         <v>-0.493676</v>
       </c>
-      <c r="I17" s="36">
+      <c r="I17" s="37">
         <v>-0.325308</v>
       </c>
-      <c r="J17" s="37">
+      <c r="J17" s="38">
         <v>-0.522784</v>
       </c>
-      <c r="K17" s="38">
+      <c r="K17" s="39">
         <v>-0.429327</v>
       </c>
-      <c r="L17" s="39">
+      <c r="L17" s="40">
         <v>-0.568155</v>
       </c>
-      <c r="M17" s="40">
+      <c r="M17" s="41">
         <v>-0.803342</v>
       </c>
       <c r="O17" s="43"/>
@@ -2025,40 +2070,40 @@
       <c r="A18" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="30">
         <v>0.009203</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="31">
         <v>0.938541</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="32">
         <v>0.790983</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="33">
         <v>0.344653</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="34">
         <v>0.897416</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="35">
         <v>0.759268</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="36">
         <v>0.448867</v>
       </c>
-      <c r="I18" s="36">
+      <c r="I18" s="37">
         <v>0.814063</v>
       </c>
-      <c r="J18" s="37">
+      <c r="J18" s="38">
         <v>0.865881</v>
       </c>
-      <c r="K18" s="38">
+      <c r="K18" s="39">
         <v>0.453786</v>
       </c>
-      <c r="L18" s="39">
+      <c r="L18" s="40">
         <v>0.73159</v>
       </c>
-      <c r="M18" s="40">
+      <c r="M18" s="41">
         <v>0.914654</v>
       </c>
       <c r="O18" s="43"/>
@@ -2081,40 +2126,40 @@
       <c r="A19" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="30">
         <v>0.147181</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="31">
         <v>0.716698</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="32">
         <v>0.588306</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="33">
         <v>0.102413</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="34">
         <v>0.631492</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="35">
         <v>-0.154611</v>
       </c>
-      <c r="H19" s="35">
+      <c r="H19" s="36">
         <v>0.248043</v>
       </c>
-      <c r="I19" s="36">
+      <c r="I19" s="37">
         <v>0.265512</v>
       </c>
-      <c r="J19" s="37">
+      <c r="J19" s="38">
         <v>0.139218</v>
       </c>
-      <c r="K19" s="38">
+      <c r="K19" s="39">
         <v>0.369732</v>
       </c>
-      <c r="L19" s="39">
+      <c r="L19" s="40">
         <v>0.325229</v>
       </c>
-      <c r="M19" s="40">
+      <c r="M19" s="41">
         <v>0.424531</v>
       </c>
       <c r="O19" s="43"/>
@@ -2137,40 +2182,40 @@
       <c r="A20" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="30">
         <v>0.191608</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="31">
         <v>0.885551</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="32">
         <v>0.806915</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="33">
         <v>0.369005</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="34">
         <v>0.815502</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="35">
         <v>0.260828</v>
       </c>
-      <c r="H20" s="35">
+      <c r="H20" s="36">
         <v>0.307311</v>
       </c>
-      <c r="I20" s="36">
+      <c r="I20" s="37">
         <v>0.530421</v>
       </c>
-      <c r="J20" s="37">
+      <c r="J20" s="38">
         <v>0.628699</v>
       </c>
-      <c r="K20" s="38">
+      <c r="K20" s="39">
         <v>0.431107</v>
       </c>
-      <c r="L20" s="39">
+      <c r="L20" s="40">
         <v>0.460101</v>
       </c>
-      <c r="M20" s="40">
+      <c r="M20" s="41">
         <v>0.714164</v>
       </c>
       <c r="O20" s="43"/>
@@ -2193,40 +2238,40 @@
       <c r="A21" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="30">
         <v>0.083401</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="31">
         <v>-0.411857</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="32">
         <v>-0.52913</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="33">
         <v>-0.122096</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="34">
         <v>-0.164599</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="35">
         <v>-0.470268</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H21" s="36">
         <v>0.168923</v>
       </c>
-      <c r="I21" s="36">
+      <c r="I21" s="37">
         <v>-0.315158</v>
       </c>
-      <c r="J21" s="37">
+      <c r="J21" s="38">
         <v>-0.575486</v>
       </c>
-      <c r="K21" s="38">
+      <c r="K21" s="39">
         <v>0.045096</v>
       </c>
-      <c r="L21" s="39">
+      <c r="L21" s="40">
         <v>0.005476</v>
       </c>
-      <c r="M21" s="40">
+      <c r="M21" s="41">
         <v>-0.538699</v>
       </c>
       <c r="O21" s="43"/>
@@ -2249,40 +2294,40 @@
       <c r="A22" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="30">
         <v>-0.109921</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="31">
         <v>-0.674837</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="32">
         <v>-0.559588</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="33">
         <v>-0.332862</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="34">
         <v>-0.45209</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="35">
         <v>-0.497947</v>
       </c>
-      <c r="H22" s="35">
+      <c r="H22" s="36">
         <v>-0.059259</v>
       </c>
-      <c r="I22" s="36">
+      <c r="I22" s="37">
         <v>-0.445912</v>
       </c>
-      <c r="J22" s="37">
+      <c r="J22" s="38">
         <v>-0.598135</v>
       </c>
-      <c r="K22" s="38">
+      <c r="K22" s="39">
         <v>-0.112913</v>
       </c>
-      <c r="L22" s="39">
+      <c r="L22" s="40">
         <v>-0.110423</v>
       </c>
-      <c r="M22" s="40">
+      <c r="M22" s="41">
         <v>-0.560123</v>
       </c>
       <c r="O22" s="43"/>
@@ -2305,41 +2350,41 @@
       <c r="A23" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="30">
         <v>-0.361376</v>
       </c>
-      <c r="C23" s="30">
-        <v>-0.507332</v>
-      </c>
-      <c r="D23" s="31">
-        <v>-0.657587</v>
-      </c>
-      <c r="E23" s="32">
+      <c r="C23" s="31">
+        <v>0.026403</v>
+      </c>
+      <c r="D23" s="32">
+        <v>-0.352707</v>
+      </c>
+      <c r="E23" s="33">
         <v>-0.17737</v>
       </c>
-      <c r="F23" s="33">
-        <v>-0.705564</v>
-      </c>
-      <c r="G23" s="34">
-        <v>-0.657882</v>
-      </c>
-      <c r="H23" s="35">
+      <c r="F23" s="34">
+        <v>-0.033176</v>
+      </c>
+      <c r="G23" s="35">
+        <v>-0.411478</v>
+      </c>
+      <c r="H23" s="36">
         <v>-0.260119</v>
       </c>
-      <c r="I23" s="36">
-        <v>-0.525312</v>
-      </c>
-      <c r="J23" s="37">
-        <v>-0.541838</v>
-      </c>
-      <c r="K23" s="38">
+      <c r="I23" s="37">
+        <v>-0.072053</v>
+      </c>
+      <c r="J23" s="38">
+        <v>-0.396916</v>
+      </c>
+      <c r="K23" s="39">
         <v>-0.214938</v>
       </c>
-      <c r="L23" s="39">
-        <v>-0.215387</v>
-      </c>
-      <c r="M23" s="40">
-        <v>-0.467013</v>
+      <c r="L23" s="40">
+        <v>-0.308342</v>
+      </c>
+      <c r="M23" s="41">
+        <v>-0.409175</v>
       </c>
       <c r="O23" s="43"/>
       <c r="P23" s="43"/>
@@ -2365,37 +2410,37 @@
         <v>-0.434821</v>
       </c>
       <c r="C24" s="48">
-        <v>-0.549578</v>
+        <v>0.006978</v>
       </c>
       <c r="D24" s="49">
-        <v>-0.682362</v>
+        <v>-0.371272</v>
       </c>
       <c r="E24" s="50">
         <v>-0.242849</v>
       </c>
       <c r="F24" s="51">
-        <v>-0.744804</v>
+        <v>-0.045842</v>
       </c>
       <c r="G24" s="52">
-        <v>-0.679929</v>
+        <v>-0.432933</v>
       </c>
       <c r="H24" s="53">
         <v>-0.34254</v>
       </c>
       <c r="I24" s="54">
-        <v>-0.597062</v>
+        <v>-0.122682</v>
       </c>
       <c r="J24" s="55">
-        <v>-0.564424</v>
+        <v>-0.415155</v>
       </c>
       <c r="K24" s="56">
         <v>-0.275058</v>
       </c>
       <c r="L24" s="57">
-        <v>-0.279152</v>
+        <v>-0.337453</v>
       </c>
       <c r="M24" s="58">
-        <v>-0.488685</v>
+        <v>-0.422961</v>
       </c>
       <c r="O24" s="43"/>
       <c r="P24" s="43"/>
@@ -2449,40 +2494,40 @@
       <c r="A26" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B26" s="30">
         <v>0.677731</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="31">
         <v>0.970603</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="32">
         <v>0.917071</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="33">
         <v>0.648214</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="34">
         <v>0.927695</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="35">
         <v>0.7562</v>
       </c>
-      <c r="H26" s="35">
+      <c r="H26" s="36">
         <v>0.451391</v>
       </c>
-      <c r="I26" s="36">
+      <c r="I26" s="37">
         <v>0.661617</v>
       </c>
-      <c r="J26" s="37">
+      <c r="J26" s="38">
         <v>0.527313</v>
       </c>
-      <c r="K26" s="38">
+      <c r="K26" s="39">
         <v>0.110564</v>
       </c>
-      <c r="L26" s="39">
+      <c r="L26" s="40">
         <v>0.17174</v>
       </c>
-      <c r="M26" s="40">
+      <c r="M26" s="41">
         <v>0.231239</v>
       </c>
       <c r="O26" s="43"/>
@@ -2505,40 +2550,40 @@
       <c r="A27" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="30">
         <v>0.737382</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="31">
         <v>0.973611</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="32">
         <v>0.939714</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="33">
         <v>0.715535</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="34">
         <v>0.907355</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="35">
         <v>0.823149</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="36">
         <v>0.353708</v>
       </c>
-      <c r="I27" s="36">
+      <c r="I27" s="37">
         <v>0.729284</v>
       </c>
-      <c r="J27" s="37">
+      <c r="J27" s="38">
         <v>0.536241</v>
       </c>
-      <c r="K27" s="38">
+      <c r="K27" s="39">
         <v>-0.048941</v>
       </c>
-      <c r="L27" s="39">
+      <c r="L27" s="40">
         <v>0.32797</v>
       </c>
-      <c r="M27" s="40">
+      <c r="M27" s="41">
         <v>0.154545</v>
       </c>
     </row>
@@ -2546,40 +2591,40 @@
       <c r="A28" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="30">
         <v>0.716267</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="31">
         <v>0.972699</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="32">
         <v>0.952578</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="33">
         <v>0.712247</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="34">
         <v>0.924472</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="35">
         <v>0.927105</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="36">
         <v>0.508811</v>
       </c>
-      <c r="I28" s="36">
+      <c r="I28" s="37">
         <v>0.651502</v>
       </c>
-      <c r="J28" s="37">
+      <c r="J28" s="38">
         <v>0.816355</v>
       </c>
-      <c r="K28" s="38">
+      <c r="K28" s="39">
         <v>0.032275</v>
       </c>
-      <c r="L28" s="39">
+      <c r="L28" s="40">
         <v>0.110047</v>
       </c>
-      <c r="M28" s="40">
+      <c r="M28" s="41">
         <v>0.476477</v>
       </c>
     </row>
@@ -2587,40 +2632,40 @@
       <c r="A29" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="30">
         <v>0.76718</v>
       </c>
-      <c r="C29" s="30">
+      <c r="C29" s="31">
         <v>0.927199</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="32">
         <v>0.757003</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="33">
         <v>0.492718</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="34">
         <v>0.866849</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="35">
         <v>0.67488</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="36">
         <v>0.267938</v>
       </c>
-      <c r="I29" s="36">
+      <c r="I29" s="37">
         <v>0.536448</v>
       </c>
-      <c r="J29" s="37">
+      <c r="J29" s="38">
         <v>0.517939</v>
       </c>
-      <c r="K29" s="38">
+      <c r="K29" s="39">
         <v>-0.046259</v>
       </c>
-      <c r="L29" s="39">
+      <c r="L29" s="40">
         <v>0.034272</v>
       </c>
-      <c r="M29" s="40">
+      <c r="M29" s="41">
         <v>0.258297</v>
       </c>
     </row>
@@ -2628,40 +2673,40 @@
       <c r="A30" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="29">
+      <c r="B30" s="30">
         <v>0.569077</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="31">
         <v>0.887175</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="32">
         <v>0.887516</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="33">
         <v>0.557472</v>
       </c>
-      <c r="F30" s="33">
+      <c r="F30" s="34">
         <v>0.852985</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="35">
         <v>0.735167</v>
       </c>
-      <c r="H30" s="35">
+      <c r="H30" s="36">
         <v>0.196882</v>
       </c>
-      <c r="I30" s="36">
+      <c r="I30" s="37">
         <v>0.371755</v>
       </c>
-      <c r="J30" s="37">
+      <c r="J30" s="38">
         <v>0.566942</v>
       </c>
-      <c r="K30" s="38">
+      <c r="K30" s="39">
         <v>-0.135994</v>
       </c>
-      <c r="L30" s="39">
+      <c r="L30" s="40">
         <v>0.086493</v>
       </c>
-      <c r="M30" s="40">
+      <c r="M30" s="41">
         <v>0.248915</v>
       </c>
     </row>
@@ -2669,40 +2714,40 @@
       <c r="A31" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="29">
+      <c r="B31" s="30">
         <v>0.782443</v>
       </c>
-      <c r="C31" s="30">
+      <c r="C31" s="31">
         <v>0.906064</v>
       </c>
-      <c r="D31" s="31">
+      <c r="D31" s="32">
         <v>0.920165</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="33">
         <v>0.725205</v>
       </c>
-      <c r="F31" s="33">
+      <c r="F31" s="34">
         <v>0.845547</v>
       </c>
-      <c r="G31" s="34">
+      <c r="G31" s="35">
         <v>0.631427</v>
       </c>
-      <c r="H31" s="35">
+      <c r="H31" s="36">
         <v>0.152285</v>
       </c>
-      <c r="I31" s="36">
+      <c r="I31" s="37">
         <v>0.468913</v>
       </c>
-      <c r="J31" s="37">
+      <c r="J31" s="38">
         <v>0.256365</v>
       </c>
-      <c r="K31" s="38">
+      <c r="K31" s="39">
         <v>-0.177399</v>
       </c>
-      <c r="L31" s="39">
+      <c r="L31" s="40">
         <v>0.111217</v>
       </c>
-      <c r="M31" s="40">
+      <c r="M31" s="41">
         <v>0.010179</v>
       </c>
     </row>
@@ -2710,40 +2755,40 @@
       <c r="A32" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="29">
+      <c r="B32" s="30">
         <v>0.692582</v>
       </c>
-      <c r="C32" s="30">
+      <c r="C32" s="31">
         <v>0.800606</v>
       </c>
-      <c r="D32" s="31">
+      <c r="D32" s="32">
         <v>0.862876</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="33">
         <v>0.499099</v>
       </c>
-      <c r="F32" s="33">
+      <c r="F32" s="34">
         <v>0.766901</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="35">
         <v>0.846806</v>
       </c>
-      <c r="H32" s="35">
+      <c r="H32" s="36">
         <v>0.051342</v>
       </c>
-      <c r="I32" s="36">
+      <c r="I32" s="37">
         <v>0.431766</v>
       </c>
-      <c r="J32" s="37">
+      <c r="J32" s="38">
         <v>0.605049</v>
       </c>
-      <c r="K32" s="38">
+      <c r="K32" s="39">
         <v>-0.153132</v>
       </c>
-      <c r="L32" s="39">
+      <c r="L32" s="40">
         <v>-0.005214</v>
       </c>
-      <c r="M32" s="40">
+      <c r="M32" s="41">
         <v>0.170594</v>
       </c>
     </row>
@@ -2755,37 +2800,37 @@
         <v>-0.019037</v>
       </c>
       <c r="C33" s="48">
-        <v>0.799164</v>
+        <v>0.378347</v>
       </c>
       <c r="D33" s="49">
-        <v>0.875962</v>
+        <v>0.807224</v>
       </c>
       <c r="E33" s="50">
         <v>-0.251017</v>
       </c>
       <c r="F33" s="51">
-        <v>0.792422</v>
+        <v>0.103681</v>
       </c>
       <c r="G33" s="52">
-        <v>0.842527</v>
+        <v>0.689046</v>
       </c>
       <c r="H33" s="53">
         <v>-0.239439</v>
       </c>
       <c r="I33" s="54">
-        <v>0.543337</v>
+        <v>0.134271</v>
       </c>
       <c r="J33" s="55">
-        <v>0.663498</v>
+        <v>0.705619</v>
       </c>
       <c r="K33" s="56">
         <v>-0.401389</v>
       </c>
       <c r="L33" s="57">
-        <v>0.031181</v>
+        <v>-0.010895</v>
       </c>
       <c r="M33" s="58">
-        <v>0.242965</v>
+        <v>0.456838</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
@@ -2818,31 +2863,31 @@
       <c r="D35" s="71">
         <v>-1.791013</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="33">
         <v>-10.761766</v>
       </c>
       <c r="F35" s="72">
         <v>-6.625162</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="35">
         <v>-1.791013</v>
       </c>
-      <c r="H35" s="35">
+      <c r="H35" s="36">
         <v>-10.761766</v>
       </c>
-      <c r="I35" s="36">
+      <c r="I35" s="37">
         <v>-6.625162</v>
       </c>
-      <c r="J35" s="37">
+      <c r="J35" s="38">
         <v>-1.791013</v>
       </c>
-      <c r="K35" s="38">
+      <c r="K35" s="39">
         <v>-10.761766</v>
       </c>
       <c r="L35" s="73">
         <v>-6.625162</v>
       </c>
-      <c r="M35" s="40">
+      <c r="M35" s="41">
         <v>-1.791013</v>
       </c>
     </row>

</xml_diff>